<commit_message>
Changed . to , in excell
</commit_message>
<xml_diff>
--- a/Experiments Hill Climbing.xlsx
+++ b/Experiments Hill Climbing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7040" yWindow="460" windowWidth="18920" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="25940" windowHeight="14720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="191">
   <si>
     <t>All experiments run on an 2,9 GHz Intel Core i7 processor</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Random Mutation: 1 package; Rotations: disabled</t>
   </si>
   <si>
-    <t>216.52</t>
-  </si>
-  <si>
     <t>125.51</t>
   </si>
   <si>
@@ -95,12 +92,6 @@
     <t>14.66</t>
   </si>
   <si>
-    <t>220.56</t>
-  </si>
-  <si>
-    <t>25.04</t>
-  </si>
-  <si>
     <t>31.73</t>
   </si>
   <si>
@@ -110,9 +101,6 @@
     <t>14.97</t>
   </si>
   <si>
-    <t>221.75</t>
-  </si>
-  <si>
     <t>99.67</t>
   </si>
   <si>
@@ -125,12 +113,6 @@
     <t>15.79</t>
   </si>
   <si>
-    <t>221.84</t>
-  </si>
-  <si>
-    <t>84.81</t>
-  </si>
-  <si>
     <t>376.0</t>
   </si>
   <si>
@@ -146,12 +128,6 @@
     <t>15.32</t>
   </si>
   <si>
-    <t>223.04</t>
-  </si>
-  <si>
-    <t>130.81</t>
-  </si>
-  <si>
     <t>93.58</t>
   </si>
   <si>
@@ -167,15 +143,9 @@
     <t>Random Mutation: 5 packages; Rotations: disabled</t>
   </si>
   <si>
-    <t>218.83</t>
-  </si>
-  <si>
     <t>1.0</t>
   </si>
   <si>
-    <t>5.07</t>
-  </si>
-  <si>
     <t>113.07</t>
   </si>
   <si>
@@ -188,9 +158,6 @@
     <t>14.15</t>
   </si>
   <si>
-    <t>222.51</t>
-  </si>
-  <si>
     <t>93.82</t>
   </si>
   <si>
@@ -203,15 +170,9 @@
     <t>15.26</t>
   </si>
   <si>
-    <t>224.16</t>
-  </si>
-  <si>
     <t>86.27</t>
   </si>
   <si>
-    <t>95.69</t>
-  </si>
-  <si>
     <t>31.51</t>
   </si>
   <si>
@@ -221,9 +182,6 @@
     <t>16.07</t>
   </si>
   <si>
-    <t>224.72</t>
-  </si>
-  <si>
     <t>82.71</t>
   </si>
   <si>
@@ -236,9 +194,6 @@
     <t>15.95</t>
   </si>
   <si>
-    <t>224.83</t>
-  </si>
-  <si>
     <t>81.29</t>
   </si>
   <si>
@@ -248,9 +203,6 @@
     <t>15.73</t>
   </si>
   <si>
-    <t>225.92</t>
-  </si>
-  <si>
     <t>77.04</t>
   </si>
   <si>
@@ -263,9 +215,6 @@
     <t>Random Mutation: 10 packages; Rotations: disabled</t>
   </si>
   <si>
-    <t>221.09</t>
-  </si>
-  <si>
     <t>102.74</t>
   </si>
   <si>
@@ -278,9 +227,6 @@
     <t>15.14</t>
   </si>
   <si>
-    <t>225.76</t>
-  </si>
-  <si>
     <t>76.85</t>
   </si>
   <si>
@@ -293,9 +239,6 @@
     <t>16.01</t>
   </si>
   <si>
-    <t>226.94</t>
-  </si>
-  <si>
     <t>72.41</t>
   </si>
   <si>
@@ -308,12 +251,6 @@
     <t>16.93</t>
   </si>
   <si>
-    <t>227.55</t>
-  </si>
-  <si>
-    <t>329.88</t>
-  </si>
-  <si>
     <t>68.15</t>
   </si>
   <si>
@@ -326,9 +263,6 @@
     <t>16.75</t>
   </si>
   <si>
-    <t>228.31</t>
-  </si>
-  <si>
     <t>64.27</t>
   </si>
   <si>
@@ -341,9 +275,6 @@
     <t>16.87</t>
   </si>
   <si>
-    <t>228.41</t>
-  </si>
-  <si>
     <t>63.45</t>
   </si>
   <si>
@@ -359,15 +290,9 @@
     <t>Random Mutation: 20 packages; Rotations: disabled</t>
   </si>
   <si>
-    <t>222.59</t>
-  </si>
-  <si>
     <t>5.0</t>
   </si>
   <si>
-    <t>24.38</t>
-  </si>
-  <si>
     <t>101.0</t>
   </si>
   <si>
@@ -383,9 +308,6 @@
     <t>15.04</t>
   </si>
   <si>
-    <t>226.79</t>
-  </si>
-  <si>
     <t>28.0</t>
   </si>
   <si>
@@ -413,12 +335,6 @@
     <t>Worst runtime (ms)</t>
   </si>
   <si>
-    <t>9.72</t>
-  </si>
-  <si>
-    <t>55.01</t>
-  </si>
-  <si>
     <t>13.0</t>
   </si>
   <si>
@@ -428,18 +344,6 @@
     <t>48.0</t>
   </si>
   <si>
-    <t>30.31</t>
-  </si>
-  <si>
-    <t>172.01</t>
-  </si>
-  <si>
-    <t>135.94</t>
-  </si>
-  <si>
-    <t>286.88</t>
-  </si>
-  <si>
     <t>41.0</t>
   </si>
   <si>
@@ -479,21 +383,6 @@
     <t>40.0</t>
   </si>
   <si>
-    <t>9.35</t>
-  </si>
-  <si>
-    <t>44.36</t>
-  </si>
-  <si>
-    <t>100.89</t>
-  </si>
-  <si>
-    <t>233.5</t>
-  </si>
-  <si>
-    <t>770.31</t>
-  </si>
-  <si>
     <t>90.0</t>
   </si>
   <si>
@@ -512,9 +401,6 @@
     <t>1642.0</t>
   </si>
   <si>
-    <t>135.3</t>
-  </si>
-  <si>
     <t>454.0</t>
   </si>
   <si>
@@ -530,18 +416,12 @@
     <t>54.0</t>
   </si>
   <si>
-    <t>160.81</t>
-  </si>
-  <si>
     <t>400.0</t>
   </si>
   <si>
     <t>62.14</t>
   </si>
   <si>
-    <t>228.58</t>
-  </si>
-  <si>
     <t>31.64</t>
   </si>
   <si>
@@ -551,15 +431,9 @@
     <t>16.78</t>
   </si>
   <si>
-    <t>229.33</t>
-  </si>
-  <si>
     <t>94.0</t>
   </si>
   <si>
-    <t>576.65</t>
-  </si>
-  <si>
     <t>1399.0</t>
   </si>
   <si>
@@ -572,9 +446,6 @@
     <t>16.98</t>
   </si>
   <si>
-    <t>230.3</t>
-  </si>
-  <si>
     <t>52.94</t>
   </si>
   <si>
@@ -590,15 +461,9 @@
     <t>69.0</t>
   </si>
   <si>
-    <t>368.85</t>
-  </si>
-  <si>
     <t>941.0</t>
   </si>
   <si>
-    <t>231.05</t>
-  </si>
-  <si>
     <t>48.3</t>
   </si>
   <si>
@@ -608,21 +473,12 @@
     <t>264.0</t>
   </si>
   <si>
-    <t>769.96</t>
-  </si>
-  <si>
     <t>1926.0</t>
   </si>
   <si>
     <t>Random Mutation: 1 package; Rotations: enabled</t>
   </si>
   <si>
-    <t>193.49</t>
-  </si>
-  <si>
-    <t>4.4</t>
-  </si>
-  <si>
     <t>31.0</t>
   </si>
   <si>
@@ -638,15 +494,9 @@
     <t>14.01</t>
   </si>
   <si>
-    <t>200.23</t>
-  </si>
-  <si>
     <t>3.0</t>
   </si>
   <si>
-    <t>30.19</t>
-  </si>
-  <si>
     <t>182.0</t>
   </si>
   <si>
@@ -662,12 +512,6 @@
     <t>14.4</t>
   </si>
   <si>
-    <t>203.95</t>
-  </si>
-  <si>
-    <t>57.99</t>
-  </si>
-  <si>
     <t>247.0</t>
   </si>
   <si>
@@ -683,15 +527,9 @@
     <t>14.32</t>
   </si>
   <si>
-    <t>205.81</t>
-  </si>
-  <si>
     <t>43.0</t>
   </si>
   <si>
-    <t>129.02</t>
-  </si>
-  <si>
     <t>365.0</t>
   </si>
   <si>
@@ -707,15 +545,9 @@
     <t>14.85</t>
   </si>
   <si>
-    <t>206.34</t>
-  </si>
-  <si>
     <t>73.0</t>
   </si>
   <si>
-    <t>309.01</t>
-  </si>
-  <si>
     <t>607.0</t>
   </si>
   <si>
@@ -731,15 +563,9 @@
     <t>14.68</t>
   </si>
   <si>
-    <t>205.51</t>
-  </si>
-  <si>
     <t>18.0</t>
   </si>
   <si>
-    <t>172.11</t>
-  </si>
-  <si>
     <t>536.0</t>
   </si>
   <si>
@@ -756,6 +582,21 @@
   </si>
   <si>
     <t>Random Mutation: 5 package; Rotations: enabled</t>
+  </si>
+  <si>
+    <t>207.01</t>
+  </si>
+  <si>
+    <t>21.89</t>
+  </si>
+  <si>
+    <t>15.48</t>
+  </si>
+  <si>
+    <t>14.49</t>
+  </si>
+  <si>
+    <t>95.0</t>
   </si>
 </sst>
 </file>
@@ -901,7 +742,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -929,9 +770,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -942,6 +780,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1223,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1262,43 +1113,43 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H5" s="13" t="s">
+      <c r="E5" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1309,38 +1160,38 @@
       <c r="B6" s="7">
         <v>233</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>14</v>
+      <c r="C6" s="16">
+        <v>216.52</v>
       </c>
       <c r="D6" s="7">
         <v>189</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>121</v>
+        <v>98</v>
+      </c>
+      <c r="F6" s="16">
+        <v>2</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="H6" s="7">
         <v>30</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" s="7">
         <v>273</v>
       </c>
       <c r="K6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="M6" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1350,38 +1201,38 @@
       <c r="B7" s="8">
         <v>233</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="17">
         <v>219</v>
       </c>
       <c r="D7" s="8">
         <v>200</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>129</v>
+        <v>95</v>
+      </c>
+      <c r="F7" s="17">
+        <v>9.7200000000000006</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="H7" s="8">
         <v>43</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J7" s="8">
         <v>210</v>
       </c>
       <c r="K7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="M7" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1391,20 +1242,20 @@
       <c r="B8" s="8">
         <v>233</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>23</v>
+      <c r="C8" s="17">
+        <v>220.56</v>
       </c>
       <c r="D8" s="8">
         <v>207</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>24</v>
+        <v>96</v>
+      </c>
+      <c r="F8" s="17">
+        <v>25.04</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
       <c r="H8" s="8">
         <v>40</v>
@@ -1416,13 +1267,13 @@
         <v>177</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1432,38 +1283,38 @@
       <c r="B9" s="9">
         <v>233</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>28</v>
+      <c r="C9" s="18">
+        <v>221.75</v>
       </c>
       <c r="D9" s="9">
         <v>205</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>130</v>
+        <v>97</v>
+      </c>
+      <c r="F9" s="18">
+        <v>55.01</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="H9" s="9">
         <v>40</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="J9" s="9">
         <v>190</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1473,38 +1324,38 @@
       <c r="B10" s="9">
         <v>233</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>33</v>
+      <c r="C10" s="18">
+        <v>221.84</v>
       </c>
       <c r="D10" s="9">
         <v>207</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>34</v>
+        <v>98</v>
+      </c>
+      <c r="F10" s="18">
+        <v>84.81</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H10" s="9">
         <v>40</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="J10" s="9">
         <v>179</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1514,39 +1365,42 @@
       <c r="B11" s="10">
         <v>234</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>40</v>
+      <c r="C11" s="19">
+        <v>223.04</v>
       </c>
       <c r="D11" s="10">
         <v>210</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>41</v>
+        <v>99</v>
+      </c>
+      <c r="F11" s="19">
+        <v>130.81</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
       <c r="H11" s="10">
         <v>22</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="J11" s="10">
         <v>172</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C12" s="15"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -1555,47 +1409,47 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H15" s="13" t="s">
+      <c r="E15" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H15" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J15" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="K15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="L15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M15" s="12" t="s">
+      <c r="M15" s="11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1606,38 +1460,38 @@
       <c r="B16" s="7">
         <v>234</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>47</v>
+      <c r="C16" s="16">
+        <v>218.83</v>
       </c>
       <c r="D16" s="7">
         <v>204</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>49</v>
+        <v>39</v>
+      </c>
+      <c r="F16" s="16">
+        <v>5.07</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
       <c r="H16" s="7">
         <v>34</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J16" s="7">
         <v>193</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1647,38 +1501,38 @@
       <c r="B17" s="8">
         <v>238</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>54</v>
+      <c r="C17" s="17">
+        <v>222.51</v>
       </c>
       <c r="D17" s="8">
         <v>206</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>134</v>
+        <v>88</v>
+      </c>
+      <c r="F17" s="17">
+        <v>30.31</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="H17" s="9">
         <v>22</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="J17" s="8">
         <v>175</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1688,38 +1542,38 @@
       <c r="B18" s="8">
         <v>238</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>59</v>
+      <c r="C18" s="17">
+        <v>224.16</v>
       </c>
       <c r="D18" s="8">
         <v>210</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>61</v>
+        <v>103</v>
+      </c>
+      <c r="F18" s="17">
+        <v>95.69</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="H18" s="9">
         <v>22</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="J18" s="8">
         <v>168</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1729,38 +1583,38 @@
       <c r="B19" s="9">
         <v>238</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>65</v>
+      <c r="C19" s="18">
+        <v>224.72</v>
       </c>
       <c r="D19" s="9">
         <v>212</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>135</v>
+        <v>99</v>
+      </c>
+      <c r="F19" s="18">
+        <v>172.01</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="H19" s="9">
         <v>22</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="J19" s="9">
         <v>150</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1770,38 +1624,38 @@
       <c r="B20" s="9">
         <v>238</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>70</v>
+      <c r="C20" s="18">
+        <v>224.83</v>
       </c>
       <c r="D20" s="9">
         <v>214</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>136</v>
+        <v>104</v>
+      </c>
+      <c r="F20" s="18">
+        <v>135.94</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="H20" s="9">
         <v>22</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="J20" s="9">
         <v>149</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1811,38 +1665,38 @@
       <c r="B21" s="10">
         <v>238</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>74</v>
+      <c r="C21" s="19">
+        <v>225.92</v>
       </c>
       <c r="D21" s="10">
         <v>210</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>137</v>
+        <v>105</v>
+      </c>
+      <c r="F21" s="19">
+        <v>286.88</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="H21" s="10">
         <v>22</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="J21" s="10">
         <v>159</v>
       </c>
-      <c r="K21" s="14">
+      <c r="K21" s="13">
         <v>31611</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1852,47 +1706,47 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H25" s="13" t="s">
+      <c r="E25" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H25" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I25" s="12" t="s">
+      <c r="I25" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J25" s="12" t="s">
+      <c r="J25" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K25" s="12" t="s">
+      <c r="K25" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L25" s="12" t="s">
+      <c r="L25" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M25" s="12" t="s">
+      <c r="M25" s="11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1903,38 +1757,38 @@
       <c r="B26" s="7">
         <v>232</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>79</v>
+      <c r="C26" s="16">
+        <v>221.09</v>
       </c>
       <c r="D26" s="7">
         <v>204</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>151</v>
+        <v>39</v>
+      </c>
+      <c r="F26" s="16">
+        <v>9.35</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>156</v>
+        <v>119</v>
       </c>
       <c r="H26" s="7">
         <v>40</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="J26" s="7">
         <v>198</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -1944,38 +1798,38 @@
       <c r="B27" s="8">
         <v>234</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>84</v>
+      <c r="C27" s="17">
+        <v>225.76</v>
       </c>
       <c r="D27" s="8">
         <v>214</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>152</v>
+        <v>116</v>
+      </c>
+      <c r="F27" s="17">
+        <v>44.36</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>157</v>
+        <v>120</v>
       </c>
       <c r="H27" s="9">
         <v>34</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="J27" s="8">
         <v>134</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -1985,38 +1839,38 @@
       <c r="B28" s="8">
         <v>235</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>89</v>
+      <c r="C28" s="17">
+        <v>226.94</v>
       </c>
       <c r="D28" s="8">
         <v>211</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>153</v>
+        <v>110</v>
+      </c>
+      <c r="F28" s="17">
+        <v>100.89</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
       <c r="H28" s="9">
         <v>34</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="J28" s="8">
         <v>167</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -2026,38 +1880,38 @@
       <c r="B29" s="9">
         <v>237</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>94</v>
+      <c r="C29" s="18">
+        <v>227.55</v>
       </c>
       <c r="D29" s="9">
         <v>212</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>95</v>
+        <v>117</v>
+      </c>
+      <c r="F29" s="18">
+        <v>329.88</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>159</v>
+        <v>122</v>
       </c>
       <c r="H29" s="9">
         <v>22</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="J29" s="9">
         <v>152</v>
       </c>
       <c r="K29" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="L29" s="15" t="s">
-        <v>98</v>
+        <v>76</v>
+      </c>
+      <c r="L29" s="14" t="s">
+        <v>77</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -2067,38 +1921,38 @@
       <c r="B30" s="9">
         <v>238</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>100</v>
+      <c r="C30" s="18">
+        <v>228.31</v>
       </c>
       <c r="D30" s="9">
         <v>216</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>154</v>
+        <v>118</v>
+      </c>
+      <c r="F30" s="18">
+        <v>233.5</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>160</v>
+        <v>123</v>
       </c>
       <c r="H30" s="9">
         <v>22</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="J30" s="9">
         <v>128</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="L30" s="9" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -2108,38 +1962,38 @@
       <c r="B31" s="10">
         <v>238</v>
       </c>
-      <c r="C31" s="14" t="s">
-        <v>105</v>
+      <c r="C31" s="19">
+        <v>228.41</v>
       </c>
       <c r="D31" s="10">
         <v>217</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>155</v>
+        <v>107</v>
+      </c>
+      <c r="F31" s="19">
+        <v>770.31</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>161</v>
+        <v>124</v>
       </c>
       <c r="H31" s="10">
         <v>22</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="J31" s="10">
         <v>118</v>
       </c>
-      <c r="K31" s="14" t="s">
-        <v>107</v>
+      <c r="K31" s="13" t="s">
+        <v>84</v>
       </c>
       <c r="L31" s="10" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -2149,47 +2003,47 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H35" s="13" t="s">
+      <c r="E35" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H35" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I35" s="12" t="s">
+      <c r="I35" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J35" s="12" t="s">
+      <c r="J35" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K35" s="12" t="s">
+      <c r="K35" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L35" s="12" t="s">
+      <c r="L35" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M35" s="12" t="s">
+      <c r="M35" s="11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2200,38 +2054,38 @@
       <c r="B36" s="7">
         <v>234</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>111</v>
+      <c r="C36" s="16">
+        <v>222.59</v>
       </c>
       <c r="D36" s="7">
         <v>210</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>113</v>
+        <v>88</v>
+      </c>
+      <c r="F36" s="16">
+        <v>24.38</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="H36" s="7">
         <v>22</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="J36" s="7">
         <v>170</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="M36" s="6" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -2241,38 +2095,38 @@
       <c r="B37" s="8">
         <v>238</v>
       </c>
-      <c r="C37" s="8" t="s">
-        <v>119</v>
+      <c r="C37" s="17">
+        <v>226.79</v>
       </c>
       <c r="D37" s="8">
         <v>207</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>162</v>
+        <v>94</v>
+      </c>
+      <c r="F37" s="17">
+        <v>135.30000000000001</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="H37" s="9">
         <v>22</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>164</v>
+        <v>126</v>
       </c>
       <c r="J37" s="8">
         <v>184</v>
       </c>
       <c r="K37" s="8" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>165</v>
+        <v>127</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>166</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -2282,38 +2136,38 @@
       <c r="B38" s="8">
         <v>238</v>
       </c>
-      <c r="C38" s="8" t="s">
-        <v>171</v>
+      <c r="C38" s="17">
+        <v>228.58</v>
       </c>
       <c r="D38" s="8">
         <v>213</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>168</v>
+        <v>129</v>
+      </c>
+      <c r="F38" s="17">
+        <v>160.81</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>169</v>
+        <v>130</v>
       </c>
       <c r="H38" s="9">
         <v>22</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>170</v>
+        <v>131</v>
       </c>
       <c r="J38" s="8">
         <v>154</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>172</v>
+        <v>132</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>173</v>
+        <v>133</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>174</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2323,38 +2177,38 @@
       <c r="B39" s="9">
         <v>238</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>175</v>
+      <c r="C39" s="18">
+        <v>229.33</v>
       </c>
       <c r="D39" s="9">
         <v>216</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>177</v>
+        <v>135</v>
+      </c>
+      <c r="F39" s="18">
+        <v>576.65</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>178</v>
+        <v>136</v>
       </c>
       <c r="H39" s="9">
         <v>22</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>179</v>
+        <v>137</v>
       </c>
       <c r="J39" s="9">
         <v>130</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="L39" s="15" t="s">
-        <v>82</v>
+        <v>138</v>
+      </c>
+      <c r="L39" s="14" t="s">
+        <v>65</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>181</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2364,38 +2218,38 @@
       <c r="B40" s="9">
         <v>238</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>182</v>
+      <c r="C40" s="18">
+        <v>230.3</v>
       </c>
       <c r="D40" s="9">
         <v>220</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>188</v>
+        <v>144</v>
+      </c>
+      <c r="F40" s="18">
+        <v>368.85</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>189</v>
+        <v>145</v>
       </c>
       <c r="H40" s="9">
         <v>22</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>183</v>
+        <v>140</v>
       </c>
       <c r="J40" s="9">
         <v>109</v>
       </c>
       <c r="K40" s="9" t="s">
-        <v>184</v>
+        <v>141</v>
       </c>
       <c r="L40" s="9" t="s">
-        <v>185</v>
+        <v>142</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>186</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -2405,38 +2259,38 @@
       <c r="B41" s="10">
         <v>238</v>
       </c>
-      <c r="C41" s="14" t="s">
-        <v>190</v>
+      <c r="C41" s="19">
+        <v>231.05</v>
       </c>
       <c r="D41" s="10">
         <v>220</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>194</v>
+        <v>148</v>
+      </c>
+      <c r="F41" s="19">
+        <v>769.96</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>195</v>
+        <v>149</v>
       </c>
       <c r="H41" s="10">
         <v>22</v>
       </c>
       <c r="I41" s="10" t="s">
-        <v>191</v>
+        <v>146</v>
       </c>
       <c r="J41" s="10">
         <v>108</v>
       </c>
-      <c r="K41" s="14" t="s">
-        <v>192</v>
+      <c r="K41" s="13" t="s">
+        <v>147</v>
       </c>
       <c r="L41" s="10" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>186</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
@@ -2446,47 +2300,47 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>196</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="12" t="s">
+      <c r="A45" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="C45" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E45" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="F45" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="G45" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H45" s="13" t="s">
+      <c r="E45" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H45" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I45" s="12" t="s">
+      <c r="I45" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J45" s="12" t="s">
+      <c r="J45" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K45" s="12" t="s">
+      <c r="K45" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L45" s="12" t="s">
+      <c r="L45" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M45" s="12" t="s">
+      <c r="M45" s="11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2497,38 +2351,38 @@
       <c r="B46" s="7">
         <v>216</v>
       </c>
-      <c r="C46" s="7" t="s">
-        <v>197</v>
+      <c r="C46" s="16">
+        <v>193.49</v>
       </c>
       <c r="D46" s="7">
         <v>173</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>198</v>
+        <v>39</v>
+      </c>
+      <c r="F46" s="16">
+        <v>4.4000000000000004</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>199</v>
+        <v>151</v>
       </c>
       <c r="H46" s="7">
         <v>124</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>200</v>
+        <v>152</v>
       </c>
       <c r="J46" s="7">
         <v>353</v>
       </c>
       <c r="K46" s="7" t="s">
-        <v>201</v>
+        <v>153</v>
       </c>
       <c r="L46" s="7" t="s">
-        <v>202</v>
+        <v>154</v>
       </c>
       <c r="M46" s="6" t="s">
-        <v>203</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -2538,38 +2392,38 @@
       <c r="B47" s="8">
         <v>218</v>
       </c>
-      <c r="C47" s="8" t="s">
-        <v>204</v>
+      <c r="C47" s="17">
+        <v>200.23</v>
       </c>
       <c r="D47" s="8">
         <v>185</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>206</v>
+        <v>156</v>
+      </c>
+      <c r="F47" s="17">
+        <v>30.19</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>207</v>
+        <v>157</v>
       </c>
       <c r="H47" s="8">
         <v>100</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>208</v>
+        <v>158</v>
       </c>
       <c r="J47" s="8">
         <v>284</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>209</v>
+        <v>159</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>210</v>
+        <v>160</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>211</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -2579,38 +2433,38 @@
       <c r="B48" s="8">
         <v>219</v>
       </c>
-      <c r="C48" s="8" t="s">
-        <v>212</v>
+      <c r="C48" s="17">
+        <v>203.95</v>
       </c>
       <c r="D48" s="8">
         <v>185</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>213</v>
+        <v>88</v>
+      </c>
+      <c r="F48" s="17">
+        <v>57.99</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>214</v>
+        <v>162</v>
       </c>
       <c r="H48" s="8">
         <v>101</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>215</v>
+        <v>163</v>
       </c>
       <c r="J48" s="8">
         <v>279</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>216</v>
+        <v>164</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>217</v>
+        <v>165</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>218</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
@@ -2620,38 +2474,38 @@
       <c r="B49" s="9">
         <v>220</v>
       </c>
-      <c r="C49" s="9" t="s">
-        <v>219</v>
+      <c r="C49" s="18">
+        <v>205.81</v>
       </c>
       <c r="D49" s="9">
         <v>190</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="F49" s="9" t="s">
-        <v>221</v>
+        <v>167</v>
+      </c>
+      <c r="F49" s="18">
+        <v>129.02000000000001</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>222</v>
+        <v>168</v>
       </c>
       <c r="H49" s="9">
         <v>100</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>223</v>
+        <v>169</v>
       </c>
       <c r="J49" s="9">
         <v>262</v>
       </c>
       <c r="K49" s="9" t="s">
-        <v>224</v>
+        <v>170</v>
       </c>
       <c r="L49" s="9" t="s">
-        <v>225</v>
+        <v>171</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>226</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
@@ -2661,38 +2515,38 @@
       <c r="B50" s="9">
         <v>221</v>
       </c>
-      <c r="C50" s="9" t="s">
-        <v>235</v>
+      <c r="C50" s="18">
+        <v>205.51</v>
       </c>
       <c r="D50" s="9">
         <v>195</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="F50" s="9" t="s">
-        <v>237</v>
+        <v>179</v>
+      </c>
+      <c r="F50" s="18">
+        <v>172.11</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>238</v>
+        <v>180</v>
       </c>
       <c r="H50" s="9">
         <v>90</v>
       </c>
       <c r="I50" s="9" t="s">
-        <v>239</v>
+        <v>181</v>
       </c>
       <c r="J50" s="9">
         <v>230</v>
       </c>
       <c r="K50" s="9" t="s">
-        <v>240</v>
+        <v>182</v>
       </c>
       <c r="L50" s="9" t="s">
-        <v>241</v>
+        <v>183</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>242</v>
+        <v>184</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
@@ -2702,38 +2556,38 @@
       <c r="B51" s="10">
         <v>222</v>
       </c>
-      <c r="C51" s="10" t="s">
-        <v>227</v>
+      <c r="C51" s="19">
+        <v>206.34</v>
       </c>
       <c r="D51" s="10">
         <v>191</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="F51" s="10" t="s">
-        <v>229</v>
+        <v>173</v>
+      </c>
+      <c r="F51" s="19">
+        <v>309.01</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>230</v>
+        <v>174</v>
       </c>
       <c r="H51" s="10">
         <v>92</v>
       </c>
       <c r="I51" s="10" t="s">
-        <v>231</v>
+        <v>175</v>
       </c>
       <c r="J51" s="10">
         <v>244</v>
       </c>
       <c r="K51" s="10" t="s">
-        <v>232</v>
+        <v>176</v>
       </c>
       <c r="L51" s="10" t="s">
-        <v>233</v>
+        <v>177</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>234</v>
+        <v>178</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
@@ -2743,47 +2597,47 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>243</v>
+        <v>185</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B55" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C55" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D55" s="12" t="s">
+      <c r="D55" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E55" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="F55" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H55" s="13" t="s">
+      <c r="E55" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H55" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I55" s="12" t="s">
+      <c r="I55" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J55" s="12" t="s">
+      <c r="J55" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K55" s="12" t="s">
+      <c r="K55" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L55" s="12" t="s">
+      <c r="L55" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M55" s="12" t="s">
+      <c r="M55" s="11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2791,24 +2645,50 @@
       <c r="A56" s="7">
         <v>10</v>
       </c>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="7"/>
-      <c r="J56" s="7"/>
-      <c r="K56" s="7"/>
-      <c r="L56" s="7"/>
-      <c r="M56" s="6"/>
+      <c r="B56" s="7">
+        <v>215</v>
+      </c>
+      <c r="C56" s="7">
+        <v>200.04</v>
+      </c>
+      <c r="D56" s="7">
+        <v>183</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F56" s="7">
+        <v>13.42</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H56" s="7">
+        <v>118</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="J56" s="7">
+        <v>302</v>
+      </c>
+      <c r="K56" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="L56" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="M56" s="6" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="8">
         <v>50</v>
       </c>
-      <c r="B57" s="8"/>
+      <c r="B57" s="8">
+        <v>223</v>
+      </c>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>

</xml_diff>

<commit_message>
Hill Climbing Experiments ABC
</commit_message>
<xml_diff>
--- a/Experiments Hill Climbing.xlsx
+++ b/Experiments Hill Climbing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25940" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="6900" yWindow="460" windowWidth="19060" windowHeight="14720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="193">
   <si>
     <t>All experiments run on an 2,9 GHz Intel Core i7 processor</t>
   </si>
@@ -584,9 +584,6 @@
     <t>Random Mutation: 5 package; Rotations: enabled</t>
   </si>
   <si>
-    <t>207.01</t>
-  </si>
-  <si>
     <t>21.89</t>
   </si>
   <si>
@@ -597,6 +594,15 @@
   </si>
   <si>
     <t>95.0</t>
+  </si>
+  <si>
+    <t>Random Mutation: 10 package; Rotations: enabled</t>
+  </si>
+  <si>
+    <t>98.6</t>
+  </si>
+  <si>
+    <t>Random Mutation: 20 package; Rotations: enabled</t>
   </si>
 </sst>
 </file>
@@ -1072,10 +1078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M61"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="O45" sqref="O45"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="K82" sqref="K82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2661,25 +2667,25 @@
         <v>13.42</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H56" s="7">
         <v>118</v>
       </c>
-      <c r="I56" s="7" t="s">
-        <v>186</v>
+      <c r="I56" s="7">
+        <v>207.01</v>
       </c>
       <c r="J56" s="7">
         <v>302</v>
       </c>
       <c r="K56" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="L56" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="L56" s="7" t="s">
+      <c r="M56" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="M56" s="6" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
@@ -2689,85 +2695,797 @@
       <c r="B57" s="8">
         <v>223</v>
       </c>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="8"/>
-      <c r="K57" s="8"/>
-      <c r="L57" s="8"/>
-      <c r="M57" s="3"/>
+      <c r="C57" s="8">
+        <v>210.96</v>
+      </c>
+      <c r="D57" s="8">
+        <v>193</v>
+      </c>
+      <c r="E57" s="8">
+        <v>27</v>
+      </c>
+      <c r="F57" s="8">
+        <v>141.6</v>
+      </c>
+      <c r="G57" s="8">
+        <v>447</v>
+      </c>
+      <c r="H57" s="8">
+        <v>83</v>
+      </c>
+      <c r="I57" s="8">
+        <v>148.79</v>
+      </c>
+      <c r="J57" s="8">
+        <v>242</v>
+      </c>
+      <c r="K57" s="8">
+        <v>23.82</v>
+      </c>
+      <c r="L57" s="8">
+        <v>15.33</v>
+      </c>
+      <c r="M57" s="3">
+        <v>15.53</v>
+      </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="8">
         <v>100</v>
       </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
-      <c r="H58" s="8"/>
-      <c r="I58" s="8"/>
-      <c r="J58" s="8"/>
-      <c r="K58" s="8"/>
-      <c r="L58" s="8"/>
-      <c r="M58" s="3"/>
+      <c r="B58" s="8">
+        <v>224</v>
+      </c>
+      <c r="C58" s="8">
+        <v>214.19</v>
+      </c>
+      <c r="D58" s="8">
+        <v>200</v>
+      </c>
+      <c r="E58" s="8">
+        <v>76</v>
+      </c>
+      <c r="F58" s="8">
+        <v>339.18</v>
+      </c>
+      <c r="G58" s="8">
+        <v>881</v>
+      </c>
+      <c r="H58" s="8">
+        <v>77</v>
+      </c>
+      <c r="I58" s="8">
+        <v>127.53</v>
+      </c>
+      <c r="J58" s="8">
+        <v>203</v>
+      </c>
+      <c r="K58" s="8">
+        <v>22.98</v>
+      </c>
+      <c r="L58" s="8">
+        <v>16.850000000000001</v>
+      </c>
+      <c r="M58" s="3">
+        <v>15.57</v>
+      </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="9">
         <v>200</v>
       </c>
-      <c r="B59" s="9"/>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
-      <c r="J59" s="9"/>
-      <c r="K59" s="9"/>
-      <c r="L59" s="9"/>
-      <c r="M59" s="4"/>
+      <c r="B59" s="9">
+        <v>231</v>
+      </c>
+      <c r="C59" s="9">
+        <v>218.33</v>
+      </c>
+      <c r="D59" s="9">
+        <v>206</v>
+      </c>
+      <c r="E59" s="9">
+        <v>149</v>
+      </c>
+      <c r="F59" s="9">
+        <v>479.82</v>
+      </c>
+      <c r="G59" s="9">
+        <v>1019</v>
+      </c>
+      <c r="H59" s="9">
+        <v>40</v>
+      </c>
+      <c r="I59" s="9">
+        <v>105.03</v>
+      </c>
+      <c r="J59" s="9">
+        <v>166</v>
+      </c>
+      <c r="K59" s="9">
+        <v>23.7</v>
+      </c>
+      <c r="L59" s="9">
+        <v>16.97</v>
+      </c>
+      <c r="M59" s="4">
+        <v>15.87</v>
+      </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="9">
         <v>250</v>
       </c>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
-      <c r="J60" s="9"/>
-      <c r="K60" s="9"/>
-      <c r="L60" s="9"/>
-      <c r="M60" s="4"/>
+      <c r="B60" s="9">
+        <v>231</v>
+      </c>
+      <c r="C60" s="9">
+        <v>218.53</v>
+      </c>
+      <c r="D60" s="9">
+        <v>209</v>
+      </c>
+      <c r="E60" s="9">
+        <v>137</v>
+      </c>
+      <c r="F60" s="9">
+        <v>595.29</v>
+      </c>
+      <c r="G60" s="9">
+        <v>1471</v>
+      </c>
+      <c r="H60" s="9">
+        <v>42</v>
+      </c>
+      <c r="I60" s="9">
+        <v>103.68</v>
+      </c>
+      <c r="J60" s="9">
+        <v>157</v>
+      </c>
+      <c r="K60" s="9">
+        <v>23.55</v>
+      </c>
+      <c r="L60" s="9">
+        <v>17.07</v>
+      </c>
+      <c r="M60" s="4">
+        <v>15.92</v>
+      </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="10">
         <v>500</v>
       </c>
-      <c r="B61" s="10"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="10"/>
-      <c r="G61" s="10"/>
-      <c r="H61" s="10"/>
-      <c r="I61" s="10"/>
-      <c r="J61" s="10"/>
-      <c r="K61" s="10"/>
-      <c r="L61" s="10"/>
-      <c r="M61" s="5"/>
+      <c r="B61" s="10">
+        <v>234</v>
+      </c>
+      <c r="C61" s="10">
+        <v>219.98</v>
+      </c>
+      <c r="D61" s="10">
+        <v>209</v>
+      </c>
+      <c r="E61" s="10">
+        <v>443</v>
+      </c>
+      <c r="F61" s="10">
+        <v>1310.5899999999999</v>
+      </c>
+      <c r="G61" s="10">
+        <v>2441</v>
+      </c>
+      <c r="H61" s="10">
+        <v>18</v>
+      </c>
+      <c r="I61" s="10">
+        <v>95.71</v>
+      </c>
+      <c r="J61" s="10">
+        <v>150</v>
+      </c>
+      <c r="K61" s="10">
+        <v>23.57</v>
+      </c>
+      <c r="L61" s="10">
+        <v>17.13</v>
+      </c>
+      <c r="M61" s="5">
+        <v>16.149999999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A65" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H65" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I65" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J65" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K65" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L65" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M65" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A66" s="7">
+        <v>10</v>
+      </c>
+      <c r="B66" s="7">
+        <v>217</v>
+      </c>
+      <c r="C66" s="7">
+        <v>200.93</v>
+      </c>
+      <c r="D66" s="7">
+        <v>184</v>
+      </c>
+      <c r="E66" s="7">
+        <v>2</v>
+      </c>
+      <c r="F66" s="7">
+        <v>21.11</v>
+      </c>
+      <c r="G66" s="7">
+        <v>191</v>
+      </c>
+      <c r="H66" s="7">
+        <v>122</v>
+      </c>
+      <c r="I66" s="7">
+        <v>202.22</v>
+      </c>
+      <c r="J66" s="7">
+        <v>289</v>
+      </c>
+      <c r="K66" s="7">
+        <v>22.45</v>
+      </c>
+      <c r="L66" s="7">
+        <v>15.52</v>
+      </c>
+      <c r="M66" s="6">
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A67" s="8">
+        <v>50</v>
+      </c>
+      <c r="B67" s="8">
+        <v>227</v>
+      </c>
+      <c r="C67" s="8">
+        <v>212.45</v>
+      </c>
+      <c r="D67" s="8">
+        <v>194</v>
+      </c>
+      <c r="E67" s="8">
+        <v>15</v>
+      </c>
+      <c r="F67" s="8">
+        <v>137.72</v>
+      </c>
+      <c r="G67" s="8">
+        <v>525</v>
+      </c>
+      <c r="H67" s="8">
+        <v>71</v>
+      </c>
+      <c r="I67" s="8">
+        <v>141.30000000000001</v>
+      </c>
+      <c r="J67" s="8">
+        <v>234</v>
+      </c>
+      <c r="K67" s="8">
+        <v>24.21</v>
+      </c>
+      <c r="L67" s="8">
+        <v>15.13</v>
+      </c>
+      <c r="M67" s="3">
+        <v>15.86</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A68" s="8">
+        <v>100</v>
+      </c>
+      <c r="B68" s="8">
+        <v>229</v>
+      </c>
+      <c r="C68" s="8">
+        <v>216.22</v>
+      </c>
+      <c r="D68" s="8">
+        <v>197</v>
+      </c>
+      <c r="E68" s="8">
+        <v>117</v>
+      </c>
+      <c r="F68" s="8">
+        <v>349.26</v>
+      </c>
+      <c r="G68" s="8">
+        <v>1022</v>
+      </c>
+      <c r="H68" s="8">
+        <v>58</v>
+      </c>
+      <c r="I68" s="8">
+        <v>119.17</v>
+      </c>
+      <c r="J68" s="8">
+        <v>202</v>
+      </c>
+      <c r="K68" s="8">
+        <v>24.95</v>
+      </c>
+      <c r="L68" s="8">
+        <v>15.93</v>
+      </c>
+      <c r="M68" s="3">
+        <v>15.53</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A69" s="9">
+        <v>200</v>
+      </c>
+      <c r="B69" s="9">
+        <v>231</v>
+      </c>
+      <c r="C69" s="9">
+        <v>219.92</v>
+      </c>
+      <c r="D69" s="9">
+        <v>208</v>
+      </c>
+      <c r="E69" s="9">
+        <v>310</v>
+      </c>
+      <c r="F69" s="9">
+        <v>701.31</v>
+      </c>
+      <c r="G69" s="9">
+        <v>1485</v>
+      </c>
+      <c r="H69" s="9">
+        <v>30</v>
+      </c>
+      <c r="I69" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="J69" s="9">
+        <v>157</v>
+      </c>
+      <c r="K69" s="9">
+        <v>25</v>
+      </c>
+      <c r="L69" s="9">
+        <v>16.18</v>
+      </c>
+      <c r="M69" s="4">
+        <v>16.04</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A70" s="9">
+        <v>250</v>
+      </c>
+      <c r="B70" s="9">
+        <v>235</v>
+      </c>
+      <c r="C70" s="9">
+        <v>220.4</v>
+      </c>
+      <c r="D70" s="9">
+        <v>205</v>
+      </c>
+      <c r="E70" s="9">
+        <v>256</v>
+      </c>
+      <c r="F70" s="9">
+        <v>929.8</v>
+      </c>
+      <c r="G70" s="9">
+        <v>1791</v>
+      </c>
+      <c r="H70" s="9">
+        <v>29</v>
+      </c>
+      <c r="I70" s="9">
+        <v>95.17</v>
+      </c>
+      <c r="J70" s="9">
+        <v>172</v>
+      </c>
+      <c r="K70" s="9">
+        <v>24.77</v>
+      </c>
+      <c r="L70" s="9">
+        <v>16.510000000000002</v>
+      </c>
+      <c r="M70" s="4">
+        <v>16.010000000000002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A71" s="10">
+        <v>500</v>
+      </c>
+      <c r="B71" s="10">
+        <v>235</v>
+      </c>
+      <c r="C71" s="10">
+        <v>222.45</v>
+      </c>
+      <c r="D71" s="10">
+        <v>212</v>
+      </c>
+      <c r="E71" s="10">
+        <v>478</v>
+      </c>
+      <c r="F71" s="10">
+        <v>1676.42</v>
+      </c>
+      <c r="G71" s="10">
+        <v>2925</v>
+      </c>
+      <c r="H71" s="10">
+        <v>34</v>
+      </c>
+      <c r="I71" s="10">
+        <v>84.7</v>
+      </c>
+      <c r="J71" s="10">
+        <v>150</v>
+      </c>
+      <c r="K71" s="10">
+        <v>24.77</v>
+      </c>
+      <c r="L71" s="10">
+        <v>16.260000000000002</v>
+      </c>
+      <c r="M71" s="5">
+        <v>16.62</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A75" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F75" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G75" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H75" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I75" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J75" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K75" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L75" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M75" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A76" s="7">
+        <v>10</v>
+      </c>
+      <c r="B76" s="7">
+        <v>218</v>
+      </c>
+      <c r="C76" s="7">
+        <v>199.86</v>
+      </c>
+      <c r="D76" s="7">
+        <v>185</v>
+      </c>
+      <c r="E76" s="7">
+        <v>7</v>
+      </c>
+      <c r="F76" s="7">
+        <v>32.840000000000003</v>
+      </c>
+      <c r="G76" s="7">
+        <v>159</v>
+      </c>
+      <c r="H76" s="7">
+        <v>110</v>
+      </c>
+      <c r="I76" s="7">
+        <v>206.82</v>
+      </c>
+      <c r="J76" s="7">
+        <v>279</v>
+      </c>
+      <c r="K76" s="7">
+        <v>20.64</v>
+      </c>
+      <c r="L76" s="7">
+        <v>15.86</v>
+      </c>
+      <c r="M76" s="6">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A77" s="8">
+        <v>50</v>
+      </c>
+      <c r="B77" s="8">
+        <v>220</v>
+      </c>
+      <c r="C77" s="8">
+        <v>209.18</v>
+      </c>
+      <c r="D77" s="8">
+        <v>194</v>
+      </c>
+      <c r="E77" s="8">
+        <v>32</v>
+      </c>
+      <c r="F77" s="8">
+        <v>215.77</v>
+      </c>
+      <c r="G77" s="8">
+        <v>637</v>
+      </c>
+      <c r="H77" s="8">
+        <v>99</v>
+      </c>
+      <c r="I77" s="8">
+        <v>158.94</v>
+      </c>
+      <c r="J77" s="8">
+        <v>235</v>
+      </c>
+      <c r="K77" s="8">
+        <v>23.52</v>
+      </c>
+      <c r="L77" s="8">
+        <v>15.08</v>
+      </c>
+      <c r="M77" s="3">
+        <v>15.66</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A78" s="8">
+        <v>100</v>
+      </c>
+      <c r="B78" s="8">
+        <v>226</v>
+      </c>
+      <c r="C78" s="8">
+        <v>212.74</v>
+      </c>
+      <c r="D78" s="8">
+        <v>197</v>
+      </c>
+      <c r="E78" s="8">
+        <v>60</v>
+      </c>
+      <c r="F78" s="8">
+        <v>313.79000000000002</v>
+      </c>
+      <c r="G78" s="8">
+        <v>645</v>
+      </c>
+      <c r="H78" s="8">
+        <v>78</v>
+      </c>
+      <c r="I78" s="8">
+        <v>140.68</v>
+      </c>
+      <c r="J78" s="8">
+        <v>217</v>
+      </c>
+      <c r="K78" s="8">
+        <v>24.38</v>
+      </c>
+      <c r="L78" s="8">
+        <v>14.75</v>
+      </c>
+      <c r="M78" s="3">
+        <v>16.12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A79" s="9">
+        <v>200</v>
+      </c>
+      <c r="B79" s="9">
+        <v>228</v>
+      </c>
+      <c r="C79" s="9">
+        <v>215.72</v>
+      </c>
+      <c r="D79" s="9">
+        <v>202</v>
+      </c>
+      <c r="E79" s="9">
+        <v>214</v>
+      </c>
+      <c r="F79" s="9">
+        <v>675.24</v>
+      </c>
+      <c r="G79" s="9">
+        <v>1226</v>
+      </c>
+      <c r="H79" s="9">
+        <v>68</v>
+      </c>
+      <c r="I79" s="9">
+        <v>125.85</v>
+      </c>
+      <c r="J79" s="9">
+        <v>200</v>
+      </c>
+      <c r="K79" s="9">
+        <v>25.29</v>
+      </c>
+      <c r="L79" s="9">
+        <v>14.3</v>
+      </c>
+      <c r="M79" s="4">
+        <v>16.53</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A80" s="9">
+        <v>250</v>
+      </c>
+      <c r="B80" s="9">
+        <v>228</v>
+      </c>
+      <c r="C80" s="9">
+        <v>216.36</v>
+      </c>
+      <c r="D80" s="9">
+        <v>206</v>
+      </c>
+      <c r="E80" s="9">
+        <v>285</v>
+      </c>
+      <c r="F80" s="9">
+        <v>917.7</v>
+      </c>
+      <c r="G80" s="9">
+        <v>2095</v>
+      </c>
+      <c r="H80" s="9">
+        <v>66</v>
+      </c>
+      <c r="I80" s="9">
+        <v>121.42</v>
+      </c>
+      <c r="J80" s="9">
+        <v>175</v>
+      </c>
+      <c r="K80" s="9">
+        <v>25.34</v>
+      </c>
+      <c r="L80" s="9">
+        <v>14.71</v>
+      </c>
+      <c r="M80" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A81" s="10">
+        <v>500</v>
+      </c>
+      <c r="B81" s="10">
+        <v>232</v>
+      </c>
+      <c r="C81" s="10">
+        <v>218.54</v>
+      </c>
+      <c r="D81" s="10">
+        <v>203</v>
+      </c>
+      <c r="E81" s="10">
+        <v>803</v>
+      </c>
+      <c r="F81" s="10">
+        <v>2739.65</v>
+      </c>
+      <c r="G81" s="10">
+        <v>4735</v>
+      </c>
+      <c r="H81" s="10">
+        <v>33</v>
+      </c>
+      <c r="I81" s="10">
+        <v>108.9</v>
+      </c>
+      <c r="J81" s="10">
+        <v>185</v>
+      </c>
+      <c r="K81" s="10">
+        <v>25.32</v>
+      </c>
+      <c r="L81" s="10">
+        <v>15.02</v>
+      </c>
+      <c r="M81" s="5">
+        <v>16.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>